<commit_message>
upload file plan 1
</commit_message>
<xml_diff>
--- a/Đăng ký đề tài/DA92_CNTT_TruongDinhTu.xlsx
+++ b/Đăng ký đề tài/DA92_CNTT_TruongDinhTu.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DACNTT2\Đăng ký đề tài\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116EC43B-A161-4099-9647-CF191D295FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Kế hoạch" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN DỰ ÁN CÔNG NGHỆ THÔNG TIN 2 - ĐỢT 1B/2021-2022</t>
   </si>
@@ -86,9 +85,6 @@
   </si>
   <si>
     <t>Tên sinh viên 2:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email: </t>
   </si>
   <si>
     <t xml:space="preserve">Tên đề tài: </t>
@@ -163,14 +159,25 @@
     <t>Nghiên cứu xây dựng hệ thống nhà thông minh điều khiển qua trợ lý ảo Google.</t>
   </si>
   <si>
-    <t>- Tìm hiểu về các thiết bị IoT
-- Tìm hiểu về google assistant</t>
+    <t>- Tìm hiểu về Internet Of Thing
+- Tìm hiểu về các thiết bị trong IoT</t>
+  </si>
+  <si>
+    <t>- Tìm hiểu về nhà thông minh.
+- Tìm hiểu về trợ lý ảo Google</t>
+  </si>
+  <si>
+    <t>- Vẽ sơ đồ thiết kế hệ điều khiển qua trợ lý ảo Google
+-….</t>
+  </si>
+  <si>
+    <t>Email:  truongdinhtu@tdtu.edu.vn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,11 +644,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -657,7 +664,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -764,7 +771,7 @@
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -800,7 +807,7 @@
         <v>51702048</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -832,7 +839,7 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -868,7 +875,7 @@
         <v>51702101</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -932,13 +939,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -965,10 +972,10 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1118,10 +1125,10 @@
         <v>33</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1144,7 +1151,7 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
     </row>
-    <row r="16" spans="1:27" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>2</v>
       </c>
@@ -1158,13 +1165,13 @@
         <v>44682</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1187,7 +1194,7 @@
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
     </row>
-    <row r="17" spans="1:27" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>3</v>
       </c>
@@ -1201,13 +1208,13 @@
         <v>44689</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1244,13 +1251,13 @@
         <v>44696</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1287,13 +1294,13 @@
         <v>44703</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -1330,13 +1337,13 @@
         <v>44710</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -1412,13 +1419,13 @@
         <v>44724</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1455,13 +1462,13 @@
         <v>44731</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -1498,13 +1505,13 @@
         <v>44738</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1541,13 +1548,13 @@
         <v>44745</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -1584,13 +1591,13 @@
         <v>44752</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -1627,13 +1634,13 @@
         <v>44759</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -1689,12 +1696,12 @@
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -29949,7 +29956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update file plan.excel 2 by Hieu
</commit_message>
<xml_diff>
--- a/Đăng ký đề tài/DA92_CNTT_TruongDinhTu.xlsx
+++ b/Đăng ký đề tài/DA92_CNTT_TruongDinhTu.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DACNTT2\Đăng ký đề tài\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DACNTT 2\DACNTT2\Đăng ký đề tài\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E717C4-1D31-479B-963C-DC040FA69F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Kế hoạch" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN DỰ ÁN CÔNG NGHỆ THÔNG TIN 2 - ĐỢT 1B/2021-2022</t>
   </si>
@@ -160,10 +159,6 @@
     <t>Nghiên cứu xây dựng hệ thống nhà thông minh điều khiển qua trợ lý ảo Google.</t>
   </si>
   <si>
-    <t>- Tìm hiểu về Internet Of Thing
-- Tìm hiểu về các thiết bị trong IoT</t>
-  </si>
-  <si>
     <t>- Tìm hiểu về nhà thông minh.
 - Tìm hiểu về trợ lý ảo Google</t>
   </si>
@@ -174,39 +169,48 @@
     <t>- Viết báo cáo</t>
   </si>
   <si>
-    <t>- Tổng hợp những thông tin tìm hiểu và viết báo cáo</t>
-  </si>
-  <si>
     <t>-
 -…</t>
   </si>
   <si>
-    <t>- Tìm hiểu về phần mềm Cisco Packet Tracer
-- Thiết kế sơ đồ điều khiển trợ lý ảo</t>
+    <t xml:space="preserve">- Tổng hợp báo cáo </t>
   </si>
   <si>
-    <t>- Mô phỏng nhà thông minh trên Cisco Packet Tracer
--</t>
+    <t>- Tổng hợp thông tin thêm vào báo cáo</t>
   </si>
   <si>
-    <t>- Tổng hợp thông tin thêm vào báo cáo
--</t>
+    <t>- Tìm hiểu về các thiết bị công nghệ áp dụng trong đồ án này
+- Vẽ sơ đồ quy trình hoạt động</t>
   </si>
   <si>
-    <t>- Thiết kế trợ lý ảo google
--….</t>
+    <t>- Kết nối trợ lý ảo google</t>
   </si>
   <si>
-    <t>- Thiết kế trợ lý ảo google</t>
+    <t>- Xây dựng hoàn chỉnh mô hình nhà thông minh</t>
   </si>
   <si>
-    <t xml:space="preserve">- Tổng hợp báo cáo </t>
+    <t>- Tìm hiểu về Blynk</t>
+  </si>
+  <si>
+    <t>- Xây dựng mô hình thực tế</t>
+  </si>
+  <si>
+    <t>- Tìm hiểu cách kết nối trợ lý ảo google</t>
+  </si>
+  <si>
+    <t>- Tìm hiểu IoT với ESP 8266</t>
+  </si>
+  <si>
+    <t>- Tìm hiểu về Internet Of Thing 
+- Ứng dụng IoT trong thực tế
+- Những ưu điểm và nhược điểm của IoT hiện nay
+- Tổng hợp những thông tin tìm hiểu và viết báo cáo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -297,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -332,6 +336,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -673,11 +680,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -685,30 +692,30 @@
     <col min="1" max="2" width="9.109375" style="1"/>
     <col min="3" max="3" width="19.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="31.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -735,7 +742,7 @@
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="2"/>
@@ -795,10 +802,10 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
@@ -863,10 +870,10 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
@@ -974,7 +981,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1137,7 +1144,7 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:27" ht="67.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>1</v>
       </c>
@@ -1151,7 +1158,7 @@
         <v>44675</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>22</v>
@@ -1180,7 +1187,7 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
     </row>
-    <row r="16" spans="1:27" ht="67.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" ht="117.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>2</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>44682</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>22</v>
@@ -1223,7 +1230,7 @@
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
     </row>
-    <row r="17" spans="1:27" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>3</v>
       </c>
@@ -1237,7 +1244,7 @@
         <v>44689</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>22</v>
@@ -1266,7 +1273,7 @@
       <c r="Z17" s="4"/>
       <c r="AA17" s="4"/>
     </row>
-    <row r="18" spans="1:27" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>4</v>
       </c>
@@ -1280,10 +1287,10 @@
         <v>44696</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>23</v>
@@ -1309,7 +1316,7 @@
       <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
     </row>
-    <row r="19" spans="1:27" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>5</v>
       </c>
@@ -1323,7 +1330,7 @@
         <v>44703</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>22</v>
@@ -1366,7 +1373,7 @@
         <v>44710</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>22</v>
@@ -1408,11 +1415,11 @@
       <c r="D21" s="9">
         <v>44717</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -1434,7 +1441,7 @@
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
     </row>
-    <row r="22" spans="1:27" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>8</v>
       </c>
@@ -1448,7 +1455,7 @@
         <v>44724</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>22</v>
@@ -1491,7 +1498,7 @@
         <v>44731</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>22</v>
@@ -1534,7 +1541,7 @@
         <v>44738</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>22</v>
@@ -1577,7 +1584,7 @@
         <v>44745</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>22</v>
@@ -1620,7 +1627,7 @@
         <v>44752</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>22</v>
@@ -1663,7 +1670,7 @@
         <v>44759</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>22</v>
@@ -1728,7 +1735,7 @@
         <v>25</v>
       </c>
       <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="12" t="s">
         <v>24</v>
       </c>
@@ -29980,12 +29987,12 @@
     <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
them image xac nhan
</commit_message>
<xml_diff>
--- a/Đăng ký đề tài/DA92_CNTT_TruongDinhTu.xlsx
+++ b/Đăng ký đề tài/DA92_CNTT_TruongDinhTu.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DACNTT 2\DACNTT2\Đăng ký đề tài\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DACNTT2\Đăng ký đề tài\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B161FD-3262-402B-892E-EBB45A03A018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kế hoạch" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN DỰ ÁN CÔNG NGHỆ THÔNG TIN 2 - ĐỢT 1B/2021-2022</t>
   </si>
@@ -206,11 +207,17 @@
 - Những ưu điểm và nhược điểm của IoT hiện nay
 - Tổng hợp những thông tin tìm hiểu và viết báo cáo</t>
   </si>
+  <si>
+    <t>Xác nhận đồng ý hướng dẫn của GVHD</t>
+  </si>
+  <si>
+    <t>Xác nhận kế hoạch của GVHD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -351,6 +358,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,6 +417,50 @@
         <a:xfrm>
           <a:off x="1" y="0"/>
           <a:ext cx="10957560" cy="3728665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91441</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>144752</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>68579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFBA462F-6233-430A-9B26-0428C04AE336}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="91441" y="4396740"/>
+          <a:ext cx="11026111" cy="2987039"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -680,10 +734,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -29992,15 +30046,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A22:R42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A22:R22"/>
+    <mergeCell ref="A42:R42"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update word 1 by Hieu
</commit_message>
<xml_diff>
--- a/Đăng ký đề tài/DA92_CNTT_TruongDinhTu.xlsx
+++ b/Đăng ký đề tài/DA92_CNTT_TruongDinhTu.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DACNTT2\Đăng ký đề tài\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DACNTT 2\DACNTT2\Đăng ký đề tài\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B161FD-3262-402B-892E-EBB45A03A018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Kế hoạch" sheetId="1" r:id="rId1"/>
@@ -217,7 +216,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -734,10 +733,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -30046,10 +30045,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A22:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:R42"/>
     </sheetView>
   </sheetViews>

</xml_diff>